<commit_message>
Add Survey Data Table
</commit_message>
<xml_diff>
--- a/NonFBOOrganized.xlsx
+++ b/NonFBOOrganized.xlsx
@@ -565,7 +565,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -580,8 +580,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -594,8 +601,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -618,32 +630,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -655,17 +648,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
@@ -945,15 +931,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P82"/>
+  <dimension ref="A1:N82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="G66" sqref="D61:G66"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>170</v>
       </c>
@@ -972,38 +958,27 @@
       <c r="F1" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="G1">
-        <v>1</v>
-      </c>
-      <c r="H1">
-        <v>2</v>
-      </c>
-      <c r="I1">
-        <v>3</v>
-      </c>
-      <c r="J1">
+      <c r="G1" s="5">
+        <v>1</v>
+      </c>
+      <c r="H1" s="5">
+        <v>2</v>
+      </c>
+      <c r="I1" s="5">
+        <v>3</v>
+      </c>
+      <c r="J1" s="5">
         <v>4</v>
       </c>
-      <c r="K1">
+      <c r="K1" s="5">
         <v>5</v>
       </c>
-      <c r="L1">
-        <v>3</v>
-      </c>
-      <c r="M1">
-        <v>1</v>
-      </c>
-      <c r="N1">
-        <v>1</v>
-      </c>
-      <c r="O1">
-        <v>2</v>
-      </c>
-      <c r="P1">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="L1" s="5">
+        <v>6</v>
+      </c>
+      <c r="N1" s="5"/>
+    </row>
+    <row r="2" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1022,38 +997,26 @@
       <c r="F2" s="2">
         <v>1</v>
       </c>
-      <c r="G2" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H2" s="5">
-        <v>2</v>
-      </c>
-      <c r="I2" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="J2" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K2" s="6">
+      <c r="G2">
+        <v>24.5</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>23.5</v>
+      </c>
+      <c r="J2">
+        <v>24.5</v>
+      </c>
+      <c r="K2">
+        <v>19.5</v>
+      </c>
+      <c r="L2">
         <v>4</v>
       </c>
-      <c r="L2">
-        <v>2</v>
-      </c>
-      <c r="M2">
-        <v>3</v>
-      </c>
-      <c r="N2">
-        <v>2</v>
-      </c>
-      <c r="O2">
-        <v>1</v>
-      </c>
-      <c r="P2">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1072,38 +1035,26 @@
       <c r="F3" s="2">
         <v>2</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3">
         <v>17</v>
       </c>
-      <c r="H3" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="I3" s="5">
+      <c r="H3">
+        <v>24.5</v>
+      </c>
+      <c r="I3">
         <v>8</v>
       </c>
-      <c r="J3" s="6">
-        <v>1</v>
-      </c>
-      <c r="K3" s="6">
-        <v>24.5</v>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>19.5</v>
       </c>
       <c r="L3">
-        <v>3</v>
-      </c>
-      <c r="M3">
-        <v>2</v>
-      </c>
-      <c r="N3">
-        <v>1</v>
-      </c>
-      <c r="O3">
-        <v>3</v>
-      </c>
-      <c r="P3">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -1122,38 +1073,26 @@
       <c r="F4" s="2">
         <v>3</v>
       </c>
-      <c r="G4" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H4" s="5">
-        <v>3</v>
-      </c>
-      <c r="I4" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="J4" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K4" s="6">
-        <v>24.5</v>
+      <c r="G4">
+        <v>24.5</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4">
+        <v>23.5</v>
+      </c>
+      <c r="J4">
+        <v>24.5</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
       </c>
       <c r="L4">
-        <v>1</v>
-      </c>
-      <c r="M4">
-        <v>3</v>
-      </c>
-      <c r="N4">
-        <v>1</v>
-      </c>
-      <c r="O4">
-        <v>2</v>
-      </c>
-      <c r="P4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -1172,38 +1111,26 @@
       <c r="F5" s="2">
         <v>4</v>
       </c>
-      <c r="G5" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H5" s="5">
-        <v>1</v>
-      </c>
-      <c r="I5" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="J5" s="6">
+      <c r="G5">
+        <v>24.5</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>23.5</v>
+      </c>
+      <c r="J5">
         <v>17</v>
       </c>
-      <c r="K5" s="6">
-        <v>24.5</v>
+      <c r="K5">
+        <v>19.5</v>
       </c>
       <c r="L5">
-        <v>3</v>
-      </c>
-      <c r="M5">
-        <v>1</v>
-      </c>
-      <c r="N5">
-        <v>1</v>
-      </c>
-      <c r="O5">
-        <v>3</v>
-      </c>
-      <c r="P5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -1222,38 +1149,26 @@
       <c r="F6" s="2">
         <v>5</v>
       </c>
-      <c r="G6" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H6" s="6">
+      <c r="G6">
+        <v>24.5</v>
+      </c>
+      <c r="H6">
         <v>10</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6">
         <v>5</v>
       </c>
-      <c r="J6" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K6" s="6">
-        <v>24.5</v>
+      <c r="J6">
+        <v>24.5</v>
+      </c>
+      <c r="K6">
+        <v>19.5</v>
       </c>
       <c r="L6">
-        <v>2</v>
-      </c>
-      <c r="M6">
-        <v>3</v>
-      </c>
-      <c r="N6">
-        <v>3</v>
-      </c>
-      <c r="O6">
-        <v>1</v>
-      </c>
-      <c r="P6">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -1272,38 +1187,26 @@
       <c r="F7" s="2">
         <v>6</v>
       </c>
-      <c r="G7" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H7" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="I7" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="J7" s="6">
-        <v>3</v>
-      </c>
-      <c r="K7" s="6">
-        <v>24.5</v>
+      <c r="G7">
+        <v>24.5</v>
+      </c>
+      <c r="H7">
+        <v>24.5</v>
+      </c>
+      <c r="I7">
+        <v>23.5</v>
+      </c>
+      <c r="J7">
+        <v>3</v>
+      </c>
+      <c r="K7">
+        <v>19.5</v>
       </c>
       <c r="L7">
-        <v>1</v>
-      </c>
-      <c r="M7">
-        <v>3</v>
-      </c>
-      <c r="N7">
-        <v>1</v>
-      </c>
-      <c r="O7">
-        <v>3</v>
-      </c>
-      <c r="P7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -1322,38 +1225,26 @@
       <c r="F8" s="2">
         <v>7</v>
       </c>
-      <c r="G8" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H8" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="I8" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="J8" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K8" s="6">
-        <v>24.5</v>
+      <c r="G8">
+        <v>24.5</v>
+      </c>
+      <c r="H8">
+        <v>24.5</v>
+      </c>
+      <c r="I8">
+        <v>23.5</v>
+      </c>
+      <c r="J8">
+        <v>24.5</v>
+      </c>
+      <c r="K8">
+        <v>19.5</v>
       </c>
       <c r="L8">
-        <v>3</v>
-      </c>
-      <c r="M8">
-        <v>1</v>
-      </c>
-      <c r="N8">
-        <v>2</v>
-      </c>
-      <c r="O8">
-        <v>1</v>
-      </c>
-      <c r="P8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -1372,38 +1263,26 @@
       <c r="F9" s="2">
         <v>8</v>
       </c>
-      <c r="G9" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H9" s="6">
+      <c r="G9">
+        <v>24.5</v>
+      </c>
+      <c r="H9">
         <v>17</v>
       </c>
-      <c r="I9" s="6">
+      <c r="I9">
         <v>16</v>
       </c>
-      <c r="J9" s="6">
+      <c r="J9">
         <v>5</v>
       </c>
-      <c r="K9" s="6">
-        <v>24.5</v>
+      <c r="K9">
+        <v>19.5</v>
       </c>
       <c r="L9">
-        <v>2</v>
-      </c>
-      <c r="M9">
-        <v>3</v>
-      </c>
-      <c r="N9">
-        <v>1</v>
-      </c>
-      <c r="O9">
-        <v>2</v>
-      </c>
-      <c r="P9">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -1422,38 +1301,26 @@
       <c r="F10" s="2">
         <v>9</v>
       </c>
-      <c r="G10" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H10" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="I10" s="6">
+      <c r="G10">
+        <v>24.5</v>
+      </c>
+      <c r="H10">
+        <v>24.5</v>
+      </c>
+      <c r="I10">
         <v>16</v>
       </c>
-      <c r="J10" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K10" s="6">
-        <v>24.5</v>
+      <c r="J10">
+        <v>24.5</v>
+      </c>
+      <c r="K10">
+        <v>19.5</v>
       </c>
       <c r="L10">
-        <v>1</v>
-      </c>
-      <c r="M10">
-        <v>2</v>
-      </c>
-      <c r="N10">
-        <v>1</v>
-      </c>
-      <c r="O10">
-        <v>1</v>
-      </c>
-      <c r="P10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>1</v>
       </c>
@@ -1472,38 +1339,26 @@
       <c r="F11" s="2">
         <v>10</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11">
         <v>12</v>
       </c>
-      <c r="H11" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="I11" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="J11" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K11" s="6">
-        <v>3</v>
+      <c r="H11">
+        <v>24.5</v>
+      </c>
+      <c r="I11">
+        <v>23.5</v>
+      </c>
+      <c r="J11">
+        <v>24.5</v>
+      </c>
+      <c r="K11">
+        <v>9</v>
       </c>
       <c r="L11">
         <v>3</v>
       </c>
-      <c r="M11">
-        <v>3</v>
-      </c>
-      <c r="N11">
-        <v>3</v>
-      </c>
-      <c r="O11">
-        <v>2</v>
-      </c>
-      <c r="P11">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>1</v>
       </c>
@@ -1522,38 +1377,26 @@
       <c r="F12" s="2">
         <v>11</v>
       </c>
-      <c r="G12" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H12" s="5">
+      <c r="G12">
+        <v>24.5</v>
+      </c>
+      <c r="H12">
         <v>7</v>
       </c>
-      <c r="I12" s="5">
-        <v>1</v>
-      </c>
-      <c r="J12" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K12" s="6">
-        <v>24.5</v>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>24.5</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
       </c>
       <c r="L12">
-        <v>2</v>
-      </c>
-      <c r="M12">
-        <v>2</v>
-      </c>
-      <c r="N12">
-        <v>1</v>
-      </c>
-      <c r="O12">
-        <v>1</v>
-      </c>
-      <c r="P12">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>1</v>
       </c>
@@ -1572,38 +1415,26 @@
       <c r="F13" s="2">
         <v>12</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13">
         <v>8</v>
       </c>
-      <c r="H13" s="7">
-        <v>24.5</v>
-      </c>
-      <c r="I13" s="7">
+      <c r="H13">
+        <v>24.5</v>
+      </c>
+      <c r="I13">
         <v>4</v>
       </c>
-      <c r="J13" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K13" s="6">
-        <v>24.5</v>
+      <c r="J13">
+        <v>24.5</v>
+      </c>
+      <c r="K13">
+        <v>19.5</v>
       </c>
       <c r="L13">
-        <v>3</v>
-      </c>
-      <c r="M13">
-        <v>1</v>
-      </c>
-      <c r="N13">
-        <v>3</v>
-      </c>
-      <c r="O13">
-        <v>1</v>
-      </c>
-      <c r="P13">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>1</v>
       </c>
@@ -1622,38 +1453,26 @@
       <c r="F14" s="2">
         <v>13</v>
       </c>
-      <c r="G14" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H14" s="7">
-        <v>24.5</v>
-      </c>
-      <c r="I14" s="7">
+      <c r="G14">
+        <v>24.5</v>
+      </c>
+      <c r="H14">
+        <v>24.5</v>
+      </c>
+      <c r="I14">
         <v>13</v>
       </c>
-      <c r="J14" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K14" s="6">
-        <v>24.5</v>
+      <c r="J14">
+        <v>24.5</v>
+      </c>
+      <c r="K14">
+        <v>19.5</v>
       </c>
       <c r="L14">
-        <v>3</v>
-      </c>
-      <c r="M14">
-        <v>3</v>
-      </c>
-      <c r="N14">
-        <v>2</v>
-      </c>
-      <c r="O14">
-        <v>3</v>
-      </c>
-      <c r="P14">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>1</v>
       </c>
@@ -1672,38 +1491,26 @@
       <c r="F15" s="2">
         <v>14</v>
       </c>
-      <c r="G15" s="5">
+      <c r="G15">
         <v>10</v>
       </c>
-      <c r="H15" s="7">
-        <v>24.5</v>
-      </c>
-      <c r="I15" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="J15" s="6">
-        <v>2</v>
-      </c>
-      <c r="K15" s="6">
-        <v>24.5</v>
+      <c r="H15">
+        <v>24.5</v>
+      </c>
+      <c r="I15">
+        <v>23.5</v>
+      </c>
+      <c r="J15">
+        <v>2</v>
+      </c>
+      <c r="K15">
+        <v>19.5</v>
       </c>
       <c r="L15">
-        <v>1</v>
-      </c>
-      <c r="M15">
-        <v>3</v>
-      </c>
-      <c r="N15">
-        <v>3</v>
-      </c>
-      <c r="O15">
-        <v>1</v>
-      </c>
-      <c r="P15">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>1</v>
       </c>
@@ -1722,38 +1529,26 @@
       <c r="F16" s="2">
         <v>15</v>
       </c>
-      <c r="G16" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H16" s="7">
-        <v>24.5</v>
-      </c>
-      <c r="I16" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="J16" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K16" s="6">
-        <v>24.5</v>
+      <c r="G16">
+        <v>24.5</v>
+      </c>
+      <c r="H16">
+        <v>24.5</v>
+      </c>
+      <c r="I16">
+        <v>23.5</v>
+      </c>
+      <c r="J16">
+        <v>24.5</v>
+      </c>
+      <c r="K16">
+        <v>6</v>
       </c>
       <c r="L16">
-        <v>3</v>
-      </c>
-      <c r="M16">
-        <v>2</v>
-      </c>
-      <c r="N16">
-        <v>2</v>
-      </c>
-      <c r="O16">
-        <v>1</v>
-      </c>
-      <c r="P16">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>1</v>
       </c>
@@ -1772,38 +1567,26 @@
       <c r="F17" s="2">
         <v>16</v>
       </c>
-      <c r="G17" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H17" s="7">
-        <v>24.5</v>
-      </c>
-      <c r="I17" s="6">
+      <c r="G17">
+        <v>24.5</v>
+      </c>
+      <c r="H17">
+        <v>24.5</v>
+      </c>
+      <c r="I17">
         <v>16</v>
       </c>
-      <c r="J17" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K17" s="6">
-        <v>24.5</v>
+      <c r="J17">
+        <v>24.5</v>
+      </c>
+      <c r="K17">
+        <v>19.5</v>
       </c>
       <c r="L17">
-        <v>1</v>
-      </c>
-      <c r="M17">
-        <v>3</v>
-      </c>
-      <c r="N17">
-        <v>2</v>
-      </c>
-      <c r="O17">
-        <v>1</v>
-      </c>
-      <c r="P17">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>1</v>
       </c>
@@ -1822,38 +1605,26 @@
       <c r="F18" s="2">
         <v>17</v>
       </c>
-      <c r="G18" s="5">
+      <c r="G18">
         <v>17</v>
       </c>
-      <c r="H18" s="5">
+      <c r="H18">
         <v>17</v>
       </c>
-      <c r="I18" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="J18" s="6">
+      <c r="I18">
+        <v>23.5</v>
+      </c>
+      <c r="J18">
         <v>8</v>
       </c>
-      <c r="K18" s="6">
-        <v>24.5</v>
+      <c r="K18">
+        <v>19.5</v>
       </c>
       <c r="L18">
-        <v>3</v>
-      </c>
-      <c r="M18">
-        <v>2</v>
-      </c>
-      <c r="N18">
-        <v>3</v>
-      </c>
-      <c r="O18">
-        <v>1</v>
-      </c>
-      <c r="P18">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>1</v>
       </c>
@@ -1872,38 +1643,26 @@
       <c r="F19" s="2">
         <v>18</v>
       </c>
-      <c r="G19" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H19" s="7">
-        <v>24.5</v>
-      </c>
-      <c r="I19" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="J19" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K19" s="6">
-        <v>24.5</v>
+      <c r="G19">
+        <v>24.5</v>
+      </c>
+      <c r="H19">
+        <v>24.5</v>
+      </c>
+      <c r="I19">
+        <v>23.5</v>
+      </c>
+      <c r="J19">
+        <v>24.5</v>
+      </c>
+      <c r="K19">
+        <v>12</v>
       </c>
       <c r="L19">
-        <v>2</v>
-      </c>
-      <c r="M19">
-        <v>3</v>
-      </c>
-      <c r="N19">
-        <v>1</v>
-      </c>
-      <c r="O19">
-        <v>3</v>
-      </c>
-      <c r="P19">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>1</v>
       </c>
@@ -1922,38 +1681,26 @@
       <c r="F20" s="2">
         <v>19</v>
       </c>
-      <c r="G20" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H20" s="7">
-        <v>24.5</v>
-      </c>
-      <c r="I20" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="J20" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K20" s="6">
-        <v>24.5</v>
+      <c r="G20">
+        <v>24.5</v>
+      </c>
+      <c r="H20">
+        <v>24.5</v>
+      </c>
+      <c r="I20">
+        <v>23.5</v>
+      </c>
+      <c r="J20">
+        <v>24.5</v>
+      </c>
+      <c r="K20">
+        <v>19.5</v>
       </c>
       <c r="L20">
-        <v>3</v>
-      </c>
-      <c r="M20">
-        <v>2</v>
-      </c>
-      <c r="N20">
-        <v>1</v>
-      </c>
-      <c r="O20">
-        <v>2</v>
-      </c>
-      <c r="P20">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>1</v>
       </c>
@@ -1972,38 +1719,26 @@
       <c r="F21" s="2">
         <v>20</v>
       </c>
-      <c r="G21" s="5">
+      <c r="G21">
         <v>6</v>
       </c>
-      <c r="H21" s="7">
-        <v>24.5</v>
-      </c>
-      <c r="I21" s="7">
-        <v>3</v>
-      </c>
-      <c r="J21" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K21" s="6">
-        <v>1</v>
+      <c r="H21">
+        <v>24.5</v>
+      </c>
+      <c r="I21">
+        <v>3</v>
+      </c>
+      <c r="J21">
+        <v>24.5</v>
+      </c>
+      <c r="K21">
+        <v>19.5</v>
       </c>
       <c r="L21">
         <v>1</v>
       </c>
-      <c r="M21">
-        <v>1</v>
-      </c>
-      <c r="N21">
-        <v>1</v>
-      </c>
-      <c r="O21">
-        <v>1</v>
-      </c>
-      <c r="P21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>1</v>
       </c>
@@ -2022,38 +1757,26 @@
       <c r="F22" s="2">
         <v>21</v>
       </c>
-      <c r="G22" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H22" s="7">
-        <v>24.5</v>
-      </c>
-      <c r="I22" s="7">
+      <c r="G22">
+        <v>24.5</v>
+      </c>
+      <c r="H22">
+        <v>24.5</v>
+      </c>
+      <c r="I22">
         <v>12</v>
       </c>
-      <c r="J22" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K22" s="6">
-        <v>2</v>
+      <c r="J22">
+        <v>24.5</v>
+      </c>
+      <c r="K22">
+        <v>7</v>
       </c>
       <c r="L22">
-        <v>3</v>
-      </c>
-      <c r="M22">
-        <v>3</v>
-      </c>
-      <c r="N22">
-        <v>2</v>
-      </c>
-      <c r="O22">
-        <v>2</v>
-      </c>
-      <c r="P22">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>1</v>
       </c>
@@ -2072,38 +1795,26 @@
       <c r="F23" s="2">
         <v>22</v>
       </c>
-      <c r="G23" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H23" s="7">
-        <v>24.5</v>
-      </c>
-      <c r="I23" s="7">
+      <c r="G23">
+        <v>24.5</v>
+      </c>
+      <c r="H23">
+        <v>24.5</v>
+      </c>
+      <c r="I23">
         <v>11</v>
       </c>
-      <c r="J23" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K23" s="6">
+      <c r="J23">
+        <v>24.5</v>
+      </c>
+      <c r="K23">
+        <v>19.5</v>
+      </c>
+      <c r="L23">
         <v>15</v>
       </c>
-      <c r="L23">
-        <v>2</v>
-      </c>
-      <c r="M23">
-        <v>1</v>
-      </c>
-      <c r="N23">
-        <v>1</v>
-      </c>
-      <c r="O23">
-        <v>1</v>
-      </c>
-      <c r="P23">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>1</v>
       </c>
@@ -2122,38 +1833,26 @@
       <c r="F24" s="2">
         <v>23</v>
       </c>
-      <c r="G24" s="5">
-        <v>2</v>
-      </c>
-      <c r="H24" s="7">
-        <v>24.5</v>
-      </c>
-      <c r="I24" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="J24" s="6">
+      <c r="G24">
+        <v>2</v>
+      </c>
+      <c r="H24">
+        <v>24.5</v>
+      </c>
+      <c r="I24">
+        <v>23.5</v>
+      </c>
+      <c r="J24">
         <v>10</v>
       </c>
-      <c r="K24" s="6">
-        <v>24.5</v>
+      <c r="K24">
+        <v>19.5</v>
       </c>
       <c r="L24">
-        <v>3</v>
-      </c>
-      <c r="M24">
-        <v>3</v>
-      </c>
-      <c r="N24">
-        <v>3</v>
-      </c>
-      <c r="O24">
-        <v>3</v>
-      </c>
-      <c r="P24">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>1</v>
       </c>
@@ -2172,23 +1871,26 @@
       <c r="F25" s="2">
         <v>24</v>
       </c>
-      <c r="G25" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H25" s="7">
-        <v>24.5</v>
-      </c>
-      <c r="I25" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="J25" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K25" s="6">
-        <v>24.5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G25">
+        <v>24.5</v>
+      </c>
+      <c r="H25">
+        <v>24.5</v>
+      </c>
+      <c r="I25">
+        <v>23.5</v>
+      </c>
+      <c r="J25">
+        <v>24.5</v>
+      </c>
+      <c r="K25">
+        <v>19.5</v>
+      </c>
+      <c r="L25">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>1</v>
       </c>
@@ -2207,38 +1909,26 @@
       <c r="F26" s="2">
         <v>25</v>
       </c>
-      <c r="G26" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H26" s="7">
-        <v>24.5</v>
-      </c>
-      <c r="I26" s="6">
+      <c r="G26">
+        <v>24.5</v>
+      </c>
+      <c r="H26">
+        <v>24.5</v>
+      </c>
+      <c r="I26">
         <v>16</v>
       </c>
-      <c r="J26" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K26" s="6">
+      <c r="J26">
+        <v>24.5</v>
+      </c>
+      <c r="K26">
+        <v>19.5</v>
+      </c>
+      <c r="L26">
         <v>17</v>
       </c>
-      <c r="L26">
-        <v>3</v>
-      </c>
-      <c r="M26">
-        <v>3</v>
-      </c>
-      <c r="N26">
-        <v>1</v>
-      </c>
-      <c r="O26">
-        <v>1</v>
-      </c>
-      <c r="P26">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>1</v>
       </c>
@@ -2257,23 +1947,26 @@
       <c r="F27" s="2">
         <v>26</v>
       </c>
-      <c r="G27" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H27" s="7">
-        <v>24.5</v>
-      </c>
-      <c r="I27" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="J27" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K27" s="6">
-        <v>24.5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G27">
+        <v>24.5</v>
+      </c>
+      <c r="H27">
+        <v>24.5</v>
+      </c>
+      <c r="I27">
+        <v>23.5</v>
+      </c>
+      <c r="J27">
+        <v>24.5</v>
+      </c>
+      <c r="K27">
+        <v>19.5</v>
+      </c>
+      <c r="L27">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>1</v>
       </c>
@@ -2292,23 +1985,26 @@
       <c r="F28" s="2">
         <v>27</v>
       </c>
-      <c r="G28" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H28" s="7">
-        <v>24.5</v>
-      </c>
-      <c r="I28" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="J28" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K28" s="6">
-        <v>24.5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G28">
+        <v>24.5</v>
+      </c>
+      <c r="H28">
+        <v>24.5</v>
+      </c>
+      <c r="I28">
+        <v>23.5</v>
+      </c>
+      <c r="J28">
+        <v>24.5</v>
+      </c>
+      <c r="K28">
+        <v>19.5</v>
+      </c>
+      <c r="L28">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>2</v>
       </c>
@@ -2327,23 +2023,26 @@
       <c r="F29" s="2">
         <v>28</v>
       </c>
-      <c r="G29" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H29" s="5">
+      <c r="G29">
+        <v>24.5</v>
+      </c>
+      <c r="H29">
         <v>17</v>
       </c>
-      <c r="I29" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="J29" s="6">
+      <c r="I29">
+        <v>23.5</v>
+      </c>
+      <c r="J29">
         <v>17</v>
       </c>
-      <c r="K29" s="6">
+      <c r="K29">
+        <v>4</v>
+      </c>
+      <c r="L29">
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>2</v>
       </c>
@@ -2362,23 +2061,26 @@
       <c r="F30" s="2">
         <v>29</v>
       </c>
-      <c r="G30" s="5">
-        <v>1</v>
-      </c>
-      <c r="H30" s="7">
-        <v>24.5</v>
-      </c>
-      <c r="I30" s="7">
+      <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="H30">
+        <v>24.5</v>
+      </c>
+      <c r="I30">
         <v>9</v>
       </c>
-      <c r="J30" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K30" s="6">
-        <v>24.5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J30">
+        <v>24.5</v>
+      </c>
+      <c r="K30">
+        <v>5</v>
+      </c>
+      <c r="L30">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>2</v>
       </c>
@@ -2397,23 +2099,26 @@
       <c r="F31" s="2">
         <v>30</v>
       </c>
-      <c r="G31" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H31" s="7">
-        <v>24.5</v>
-      </c>
-      <c r="I31" s="7">
+      <c r="G31">
+        <v>24.5</v>
+      </c>
+      <c r="H31">
+        <v>24.5</v>
+      </c>
+      <c r="I31">
         <v>7</v>
       </c>
-      <c r="J31" s="6">
+      <c r="J31">
         <v>7</v>
       </c>
-      <c r="K31" s="6">
-        <v>24.5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K31">
+        <v>19.5</v>
+      </c>
+      <c r="L31">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>2</v>
       </c>
@@ -2432,23 +2137,26 @@
       <c r="F32" s="2">
         <v>31</v>
       </c>
-      <c r="G32" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H32" s="7">
-        <v>24.5</v>
-      </c>
-      <c r="I32" s="7">
+      <c r="G32">
+        <v>24.5</v>
+      </c>
+      <c r="H32">
+        <v>24.5</v>
+      </c>
+      <c r="I32">
         <v>16</v>
       </c>
-      <c r="J32" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K32" s="6">
-        <v>24.5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J32">
+        <v>24.5</v>
+      </c>
+      <c r="K32">
+        <v>19.5</v>
+      </c>
+      <c r="L32">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>2</v>
       </c>
@@ -2467,23 +2175,26 @@
       <c r="F33" s="2">
         <v>32</v>
       </c>
-      <c r="G33" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H33" s="5">
+      <c r="G33">
+        <v>24.5</v>
+      </c>
+      <c r="H33">
         <v>12</v>
       </c>
-      <c r="I33" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="J33" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K33" s="6">
-        <v>24.5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I33">
+        <v>23.5</v>
+      </c>
+      <c r="J33">
+        <v>24.5</v>
+      </c>
+      <c r="K33">
+        <v>19.5</v>
+      </c>
+      <c r="L33">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>2</v>
       </c>
@@ -2502,23 +2213,26 @@
       <c r="F34" s="2">
         <v>33</v>
       </c>
-      <c r="G34" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H34" s="7">
-        <v>24.5</v>
-      </c>
-      <c r="I34" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="J34" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K34" s="6">
-        <v>24.5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G34">
+        <v>24.5</v>
+      </c>
+      <c r="H34">
+        <v>24.5</v>
+      </c>
+      <c r="I34">
+        <v>23.5</v>
+      </c>
+      <c r="J34">
+        <v>24.5</v>
+      </c>
+      <c r="K34">
+        <v>12</v>
+      </c>
+      <c r="L34">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>2</v>
       </c>
@@ -2537,23 +2251,26 @@
       <c r="F35" s="2">
         <v>34</v>
       </c>
-      <c r="G35" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H35" s="7">
-        <v>24.5</v>
-      </c>
-      <c r="I35" s="6">
+      <c r="G35">
+        <v>24.5</v>
+      </c>
+      <c r="H35">
+        <v>24.5</v>
+      </c>
+      <c r="I35">
         <v>16</v>
       </c>
-      <c r="J35" s="6">
+      <c r="J35">
         <v>17</v>
       </c>
-      <c r="K35" s="6">
-        <v>24.5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K35">
+        <v>19.5</v>
+      </c>
+      <c r="L35">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>2</v>
       </c>
@@ -2572,23 +2289,26 @@
       <c r="F36" s="2">
         <v>35</v>
       </c>
-      <c r="G36" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H36" s="5">
+      <c r="G36">
+        <v>24.5</v>
+      </c>
+      <c r="H36">
         <v>17</v>
       </c>
-      <c r="I36" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="J36" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K36" s="6">
-        <v>24.5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I36">
+        <v>23.5</v>
+      </c>
+      <c r="J36">
+        <v>24.5</v>
+      </c>
+      <c r="K36">
+        <v>19.5</v>
+      </c>
+      <c r="L36">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>2</v>
       </c>
@@ -2607,23 +2327,26 @@
       <c r="F37" s="2">
         <v>36</v>
       </c>
-      <c r="G37" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H37" s="7">
-        <v>24.5</v>
-      </c>
-      <c r="I37" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="J37" s="6">
+      <c r="G37">
+        <v>24.5</v>
+      </c>
+      <c r="H37">
+        <v>24.5</v>
+      </c>
+      <c r="I37">
+        <v>23.5</v>
+      </c>
+      <c r="J37">
         <v>11</v>
       </c>
-      <c r="K37" s="6">
-        <v>24.5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K37">
+        <v>12</v>
+      </c>
+      <c r="L37">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>2</v>
       </c>
@@ -2642,23 +2365,26 @@
       <c r="F38" s="2">
         <v>37</v>
       </c>
-      <c r="G38" s="5">
+      <c r="G38">
         <v>17</v>
       </c>
-      <c r="H38" s="7">
-        <v>24.5</v>
-      </c>
-      <c r="I38" s="7">
+      <c r="H38">
+        <v>24.5</v>
+      </c>
+      <c r="I38">
         <v>6</v>
       </c>
-      <c r="J38" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K38" s="6">
+      <c r="J38">
+        <v>24.5</v>
+      </c>
+      <c r="K38">
+        <v>19.5</v>
+      </c>
+      <c r="L38">
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>2</v>
       </c>
@@ -2677,23 +2403,26 @@
       <c r="F39" s="2">
         <v>38</v>
       </c>
-      <c r="G39" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H39" s="5">
+      <c r="G39">
+        <v>24.5</v>
+      </c>
+      <c r="H39">
         <v>4</v>
       </c>
-      <c r="I39" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="J39" s="6">
+      <c r="I39">
+        <v>23.5</v>
+      </c>
+      <c r="J39">
         <v>17</v>
       </c>
-      <c r="K39" s="6">
-        <v>24.5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K39">
+        <v>19.5</v>
+      </c>
+      <c r="L39">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>2</v>
       </c>
@@ -2712,23 +2441,26 @@
       <c r="F40" s="2">
         <v>39</v>
       </c>
-      <c r="G40" s="5">
-        <v>3</v>
-      </c>
-      <c r="H40" s="7">
-        <v>24.5</v>
-      </c>
-      <c r="I40" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="J40" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K40" s="6">
-        <v>24.5</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G40">
+        <v>3</v>
+      </c>
+      <c r="H40">
+        <v>24.5</v>
+      </c>
+      <c r="I40">
+        <v>23.5</v>
+      </c>
+      <c r="J40">
+        <v>24.5</v>
+      </c>
+      <c r="K40">
+        <v>19.5</v>
+      </c>
+      <c r="L40">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>2</v>
       </c>
@@ -2747,23 +2479,26 @@
       <c r="F41" s="2">
         <v>40</v>
       </c>
-      <c r="G41" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H41" s="7">
-        <v>24.5</v>
-      </c>
-      <c r="I41" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="J41" s="6">
+      <c r="G41">
+        <v>24.5</v>
+      </c>
+      <c r="H41">
+        <v>24.5</v>
+      </c>
+      <c r="I41">
+        <v>23.5</v>
+      </c>
+      <c r="J41">
         <v>17</v>
       </c>
-      <c r="K41" s="6">
-        <v>24.5</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K41">
+        <v>12</v>
+      </c>
+      <c r="L41">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>2</v>
       </c>
@@ -2782,23 +2517,26 @@
       <c r="F42" s="2">
         <v>41</v>
       </c>
-      <c r="G42" s="5">
+      <c r="G42">
         <v>16</v>
       </c>
-      <c r="H42" s="7">
-        <v>24.5</v>
-      </c>
-      <c r="I42" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="J42" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K42" s="6">
-        <v>24.5</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H42">
+        <v>24.5</v>
+      </c>
+      <c r="I42">
+        <v>23.5</v>
+      </c>
+      <c r="J42">
+        <v>24.5</v>
+      </c>
+      <c r="K42">
+        <v>8</v>
+      </c>
+      <c r="L42">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>2</v>
       </c>
@@ -2817,23 +2555,26 @@
       <c r="F43" s="2">
         <v>42</v>
       </c>
-      <c r="G43" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H43" s="7">
-        <v>24.5</v>
-      </c>
-      <c r="I43" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="J43" s="6">
+      <c r="G43">
+        <v>24.5</v>
+      </c>
+      <c r="H43">
+        <v>24.5</v>
+      </c>
+      <c r="I43">
+        <v>23.5</v>
+      </c>
+      <c r="J43">
         <v>16</v>
       </c>
-      <c r="K43" s="6">
-        <v>24.5</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K43">
+        <v>19.5</v>
+      </c>
+      <c r="L43">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>2</v>
       </c>
@@ -2852,23 +2593,26 @@
       <c r="F44" s="2">
         <v>43</v>
       </c>
-      <c r="G44" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H44" s="7">
-        <v>24.5</v>
-      </c>
-      <c r="I44" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="J44" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K44" s="6">
-        <v>24.5</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G44">
+        <v>24.5</v>
+      </c>
+      <c r="H44">
+        <v>24.5</v>
+      </c>
+      <c r="I44">
+        <v>23.5</v>
+      </c>
+      <c r="J44">
+        <v>24.5</v>
+      </c>
+      <c r="K44">
+        <v>12</v>
+      </c>
+      <c r="L44">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>2</v>
       </c>
@@ -2887,23 +2631,26 @@
       <c r="F45" s="2">
         <v>44</v>
       </c>
-      <c r="G45" s="5">
+      <c r="G45">
         <v>11</v>
       </c>
-      <c r="H45" s="7">
-        <v>24.5</v>
-      </c>
-      <c r="I45" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="J45" s="6">
+      <c r="H45">
+        <v>24.5</v>
+      </c>
+      <c r="I45">
+        <v>23.5</v>
+      </c>
+      <c r="J45">
         <v>15</v>
       </c>
-      <c r="K45" s="6">
-        <v>24.5</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K45">
+        <v>12</v>
+      </c>
+      <c r="L45">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>2</v>
       </c>
@@ -2922,23 +2669,26 @@
       <c r="F46" s="2">
         <v>45</v>
       </c>
-      <c r="G46" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H46" s="7">
-        <v>24.5</v>
-      </c>
-      <c r="I46" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="J46" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K46" s="6">
-        <v>24.5</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G46">
+        <v>24.5</v>
+      </c>
+      <c r="H46">
+        <v>24.5</v>
+      </c>
+      <c r="I46">
+        <v>23.5</v>
+      </c>
+      <c r="J46">
+        <v>24.5</v>
+      </c>
+      <c r="K46">
+        <v>19.5</v>
+      </c>
+      <c r="L46">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>2</v>
       </c>
@@ -2957,23 +2707,26 @@
       <c r="F47" s="2">
         <v>46</v>
       </c>
-      <c r="G47" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H47" s="7">
-        <v>24.5</v>
-      </c>
-      <c r="I47" s="7">
+      <c r="G47">
+        <v>24.5</v>
+      </c>
+      <c r="H47">
+        <v>24.5</v>
+      </c>
+      <c r="I47">
         <v>14</v>
       </c>
-      <c r="J47" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K47" s="6">
-        <v>24.5</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J47">
+        <v>24.5</v>
+      </c>
+      <c r="K47">
+        <v>12</v>
+      </c>
+      <c r="L47">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>2</v>
       </c>
@@ -2992,23 +2745,26 @@
       <c r="F48" s="2">
         <v>47</v>
       </c>
-      <c r="G48" s="5">
+      <c r="G48">
         <v>17</v>
       </c>
-      <c r="H48" s="5">
+      <c r="H48">
         <v>5</v>
       </c>
-      <c r="I48" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="J48" s="6">
+      <c r="I48">
+        <v>23.5</v>
+      </c>
+      <c r="J48">
         <v>12</v>
       </c>
-      <c r="K48" s="6">
+      <c r="K48">
+        <v>3</v>
+      </c>
+      <c r="L48">
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>2</v>
       </c>
@@ -3027,23 +2783,26 @@
       <c r="F49" s="2">
         <v>48</v>
       </c>
-      <c r="G49" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H49" s="7">
-        <v>24.5</v>
-      </c>
-      <c r="I49" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="J49" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K49" s="6">
+      <c r="G49">
+        <v>24.5</v>
+      </c>
+      <c r="H49">
+        <v>24.5</v>
+      </c>
+      <c r="I49">
+        <v>23.5</v>
+      </c>
+      <c r="J49">
+        <v>24.5</v>
+      </c>
+      <c r="K49">
+        <v>19.5</v>
+      </c>
+      <c r="L49">
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>2</v>
       </c>
@@ -3062,23 +2821,26 @@
       <c r="F50" s="2">
         <v>49</v>
       </c>
-      <c r="G50" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H50" s="7">
-        <v>24.5</v>
-      </c>
-      <c r="I50" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="J50" s="6">
+      <c r="G50">
+        <v>24.5</v>
+      </c>
+      <c r="H50">
+        <v>24.5</v>
+      </c>
+      <c r="I50">
+        <v>23.5</v>
+      </c>
+      <c r="J50">
         <v>17</v>
       </c>
-      <c r="K50" s="6">
+      <c r="K50">
+        <v>19.5</v>
+      </c>
+      <c r="L50">
         <v>17</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>2</v>
       </c>
@@ -3097,23 +2859,26 @@
       <c r="F51" s="2">
         <v>50</v>
       </c>
-      <c r="G51" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H51" s="7">
-        <v>24.5</v>
-      </c>
-      <c r="I51" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="J51" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K51" s="6">
-        <v>24.5</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G51">
+        <v>24.5</v>
+      </c>
+      <c r="H51">
+        <v>24.5</v>
+      </c>
+      <c r="I51">
+        <v>23.5</v>
+      </c>
+      <c r="J51">
+        <v>24.5</v>
+      </c>
+      <c r="K51">
+        <v>19.5</v>
+      </c>
+      <c r="L51">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>2</v>
       </c>
@@ -3132,23 +2897,26 @@
       <c r="F52" s="2">
         <v>51</v>
       </c>
-      <c r="G52" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H52" s="7">
-        <v>24.5</v>
-      </c>
-      <c r="I52" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="J52" s="6">
+      <c r="G52">
+        <v>24.5</v>
+      </c>
+      <c r="H52">
+        <v>24.5</v>
+      </c>
+      <c r="I52">
+        <v>23.5</v>
+      </c>
+      <c r="J52">
         <v>17</v>
       </c>
-      <c r="K52" s="6">
-        <v>24.5</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K52">
+        <v>12</v>
+      </c>
+      <c r="L52">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>2</v>
       </c>
@@ -3167,23 +2935,26 @@
       <c r="F53" s="2">
         <v>52</v>
       </c>
-      <c r="G53" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H53" s="7">
-        <v>24.5</v>
-      </c>
-      <c r="I53" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="J53" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K53" s="6">
+      <c r="G53">
+        <v>24.5</v>
+      </c>
+      <c r="H53">
+        <v>24.5</v>
+      </c>
+      <c r="I53">
+        <v>23.5</v>
+      </c>
+      <c r="J53">
+        <v>24.5</v>
+      </c>
+      <c r="K53">
+        <v>19.5</v>
+      </c>
+      <c r="L53">
         <v>17</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>2</v>
       </c>
@@ -3202,23 +2973,26 @@
       <c r="F54" s="2">
         <v>53</v>
       </c>
-      <c r="G54" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H54" s="7">
-        <v>24.5</v>
-      </c>
-      <c r="I54" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="J54" s="6">
+      <c r="G54">
+        <v>24.5</v>
+      </c>
+      <c r="H54">
+        <v>24.5</v>
+      </c>
+      <c r="I54">
+        <v>23.5</v>
+      </c>
+      <c r="J54">
         <v>17</v>
       </c>
-      <c r="K54" s="6">
-        <v>24.5</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K54">
+        <v>19.5</v>
+      </c>
+      <c r="L54">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>2</v>
       </c>
@@ -3237,23 +3011,26 @@
       <c r="F55" s="2">
         <v>54</v>
       </c>
-      <c r="G55" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H55" s="7">
-        <v>24.5</v>
-      </c>
-      <c r="I55" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="J55" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K55" s="6">
-        <v>24.5</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G55">
+        <v>24.5</v>
+      </c>
+      <c r="H55">
+        <v>24.5</v>
+      </c>
+      <c r="I55">
+        <v>23.5</v>
+      </c>
+      <c r="J55">
+        <v>24.5</v>
+      </c>
+      <c r="K55">
+        <v>12</v>
+      </c>
+      <c r="L55">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>3</v>
       </c>
@@ -3272,23 +3049,26 @@
       <c r="F56" s="2">
         <v>55</v>
       </c>
-      <c r="G56" s="5">
+      <c r="G56">
         <v>9</v>
       </c>
-      <c r="H56" s="7">
-        <v>24.5</v>
-      </c>
-      <c r="I56" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="J56" s="6">
+      <c r="H56">
+        <v>24.5</v>
+      </c>
+      <c r="I56">
+        <v>23.5</v>
+      </c>
+      <c r="J56">
         <v>4</v>
       </c>
-      <c r="K56" s="6">
-        <v>24.5</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K56">
+        <v>19.5</v>
+      </c>
+      <c r="L56">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>3</v>
       </c>
@@ -3307,23 +3087,26 @@
       <c r="F57" s="2">
         <v>56</v>
       </c>
-      <c r="G57" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H57" s="7">
-        <v>24.5</v>
-      </c>
-      <c r="I57" s="7">
+      <c r="G57">
+        <v>24.5</v>
+      </c>
+      <c r="H57">
+        <v>24.5</v>
+      </c>
+      <c r="I57">
         <v>10</v>
       </c>
-      <c r="J57" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K57" s="6">
+      <c r="J57">
+        <v>24.5</v>
+      </c>
+      <c r="K57">
+        <v>19.5</v>
+      </c>
+      <c r="L57">
         <v>17</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>3</v>
       </c>
@@ -3342,23 +3125,26 @@
       <c r="F58" s="2">
         <v>57</v>
       </c>
-      <c r="G58" s="5">
+      <c r="G58">
         <v>4</v>
       </c>
-      <c r="H58" s="5">
+      <c r="H58">
         <v>11</v>
       </c>
-      <c r="I58" s="5">
+      <c r="I58">
         <v>15</v>
       </c>
-      <c r="J58" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K58" s="6">
+      <c r="J58">
+        <v>24.5</v>
+      </c>
+      <c r="K58">
+        <v>11</v>
+      </c>
+      <c r="L58">
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>3</v>
       </c>
@@ -3377,23 +3163,26 @@
       <c r="F59" s="2">
         <v>58</v>
       </c>
-      <c r="G59" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H59" s="7">
-        <v>24.5</v>
-      </c>
-      <c r="I59" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="J59" s="6">
+      <c r="G59">
+        <v>24.5</v>
+      </c>
+      <c r="H59">
+        <v>24.5</v>
+      </c>
+      <c r="I59">
+        <v>23.5</v>
+      </c>
+      <c r="J59">
         <v>17</v>
       </c>
-      <c r="K59" s="6">
+      <c r="K59">
+        <v>19.5</v>
+      </c>
+      <c r="L59">
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>3</v>
       </c>
@@ -3412,23 +3201,26 @@
       <c r="F60" s="2">
         <v>59</v>
       </c>
-      <c r="G60" s="5">
+      <c r="G60">
         <v>17</v>
       </c>
-      <c r="H60" s="7">
-        <v>24.5</v>
-      </c>
-      <c r="I60" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="J60" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K60" s="6">
-        <v>24.5</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H60">
+        <v>24.5</v>
+      </c>
+      <c r="I60">
+        <v>23.5</v>
+      </c>
+      <c r="J60">
+        <v>24.5</v>
+      </c>
+      <c r="K60">
+        <v>19.5</v>
+      </c>
+      <c r="L60">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>3</v>
       </c>
@@ -3447,23 +3239,26 @@
       <c r="F61" s="2">
         <v>60</v>
       </c>
-      <c r="G61" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H61" s="5">
+      <c r="G61">
+        <v>24.5</v>
+      </c>
+      <c r="H61">
         <v>6</v>
       </c>
-      <c r="I61" s="6">
+      <c r="I61">
         <v>24</v>
       </c>
-      <c r="J61" s="6">
+      <c r="J61">
         <v>14</v>
       </c>
-      <c r="K61" s="6">
-        <v>24.5</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K61">
+        <v>19.5</v>
+      </c>
+      <c r="L61">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>3</v>
       </c>
@@ -3482,23 +3277,26 @@
       <c r="F62" s="2">
         <v>61</v>
       </c>
-      <c r="G62" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H62" s="5">
+      <c r="G62">
+        <v>24.5</v>
+      </c>
+      <c r="H62">
         <v>17</v>
       </c>
-      <c r="I62" s="5">
+      <c r="I62">
         <v>16</v>
       </c>
-      <c r="J62" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K62" s="6">
+      <c r="J62">
+        <v>24.5</v>
+      </c>
+      <c r="K62">
+        <v>19.5</v>
+      </c>
+      <c r="L62">
         <v>17</v>
       </c>
     </row>
-    <row r="63" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>3</v>
       </c>
@@ -3517,23 +3315,26 @@
       <c r="F63" s="2">
         <v>62</v>
       </c>
-      <c r="G63" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H63" s="7">
-        <v>24.5</v>
-      </c>
-      <c r="I63" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="J63" s="6">
+      <c r="G63">
+        <v>24.5</v>
+      </c>
+      <c r="H63">
+        <v>24.5</v>
+      </c>
+      <c r="I63">
+        <v>23.5</v>
+      </c>
+      <c r="J63">
         <v>6</v>
       </c>
-      <c r="K63" s="6">
-        <v>24.5</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K63">
+        <v>19.5</v>
+      </c>
+      <c r="L63">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>3</v>
       </c>
@@ -3552,23 +3353,26 @@
       <c r="F64" s="2">
         <v>63</v>
       </c>
-      <c r="G64" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H64" s="5">
+      <c r="G64">
+        <v>24.5</v>
+      </c>
+      <c r="H64">
         <v>17</v>
       </c>
-      <c r="I64" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="J64" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K64" s="6">
-        <v>24.5</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I64">
+        <v>23.5</v>
+      </c>
+      <c r="J64">
+        <v>24.5</v>
+      </c>
+      <c r="K64">
+        <v>19.5</v>
+      </c>
+      <c r="L64">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>3</v>
       </c>
@@ -3587,23 +3391,26 @@
       <c r="F65" s="2">
         <v>64</v>
       </c>
-      <c r="G65" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H65" s="5">
+      <c r="G65">
+        <v>24.5</v>
+      </c>
+      <c r="H65">
         <v>17</v>
       </c>
-      <c r="I65" s="5">
+      <c r="I65">
         <v>16</v>
       </c>
-      <c r="J65" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K65" s="6">
-        <v>24.5</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J65">
+        <v>24.5</v>
+      </c>
+      <c r="K65">
+        <v>12</v>
+      </c>
+      <c r="L65">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>3</v>
       </c>
@@ -3622,23 +3429,26 @@
       <c r="F66" s="2">
         <v>65</v>
       </c>
-      <c r="G66" s="5">
+      <c r="G66">
         <v>5</v>
       </c>
-      <c r="H66" s="7">
-        <v>24.5</v>
-      </c>
-      <c r="I66" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="J66" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K66" s="6">
+      <c r="H66">
+        <v>24.5</v>
+      </c>
+      <c r="I66">
+        <v>23.5</v>
+      </c>
+      <c r="J66">
+        <v>24.5</v>
+      </c>
+      <c r="K66">
         <v>12</v>
       </c>
-    </row>
-    <row r="67" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="L66">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>3</v>
       </c>
@@ -3657,23 +3467,26 @@
       <c r="F67" s="2">
         <v>66</v>
       </c>
-      <c r="G67" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H67" s="5">
+      <c r="G67">
+        <v>24.5</v>
+      </c>
+      <c r="H67">
         <v>9</v>
       </c>
-      <c r="I67" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="J67" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K67" s="6">
+      <c r="I67">
+        <v>23.5</v>
+      </c>
+      <c r="J67">
+        <v>24.5</v>
+      </c>
+      <c r="K67">
+        <v>19.5</v>
+      </c>
+      <c r="L67">
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>3</v>
       </c>
@@ -3692,23 +3505,26 @@
       <c r="F68" s="2">
         <v>67</v>
       </c>
-      <c r="G68" s="5">
+      <c r="G68">
         <v>17</v>
       </c>
-      <c r="H68" s="7">
-        <v>24.5</v>
-      </c>
-      <c r="I68" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="J68" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K68" s="6">
+      <c r="H68">
+        <v>24.5</v>
+      </c>
+      <c r="I68">
+        <v>23.5</v>
+      </c>
+      <c r="J68">
+        <v>24.5</v>
+      </c>
+      <c r="K68">
+        <v>19.5</v>
+      </c>
+      <c r="L68">
         <v>17</v>
       </c>
     </row>
-    <row r="69" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>3</v>
       </c>
@@ -3727,23 +3543,26 @@
       <c r="F69" s="2">
         <v>68</v>
       </c>
-      <c r="G69" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H69" s="5">
+      <c r="G69">
+        <v>24.5</v>
+      </c>
+      <c r="H69">
         <v>8</v>
       </c>
-      <c r="I69" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="J69" s="6">
+      <c r="I69">
+        <v>23.5</v>
+      </c>
+      <c r="J69">
         <v>9</v>
       </c>
-      <c r="K69" s="6">
-        <v>24.5</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K69">
+        <v>19.5</v>
+      </c>
+      <c r="L69">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>3</v>
       </c>
@@ -3762,23 +3581,26 @@
       <c r="F70" s="2">
         <v>69</v>
       </c>
-      <c r="G70" s="5">
+      <c r="G70">
         <v>17</v>
       </c>
-      <c r="H70" s="7">
-        <v>24.5</v>
-      </c>
-      <c r="I70" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="J70" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K70" s="6">
-        <v>24.5</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H70">
+        <v>24.5</v>
+      </c>
+      <c r="I70">
+        <v>23.5</v>
+      </c>
+      <c r="J70">
+        <v>24.5</v>
+      </c>
+      <c r="K70">
+        <v>12</v>
+      </c>
+      <c r="L70">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>3</v>
       </c>
@@ -3797,23 +3619,26 @@
       <c r="F71" s="2">
         <v>70</v>
       </c>
-      <c r="G71" s="5">
+      <c r="G71">
         <v>17</v>
       </c>
-      <c r="H71" s="7">
-        <v>24.5</v>
-      </c>
-      <c r="I71" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="J71" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K71" s="6">
+      <c r="H71">
+        <v>24.5</v>
+      </c>
+      <c r="I71">
+        <v>23.5</v>
+      </c>
+      <c r="J71">
+        <v>24.5</v>
+      </c>
+      <c r="K71">
+        <v>19.5</v>
+      </c>
+      <c r="L71">
         <v>17</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>3</v>
       </c>
@@ -3832,23 +3657,26 @@
       <c r="F72" s="2">
         <v>71</v>
       </c>
-      <c r="G72" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H72" s="5">
+      <c r="G72">
+        <v>24.5</v>
+      </c>
+      <c r="H72">
         <v>17</v>
       </c>
-      <c r="I72" s="5">
-        <v>2</v>
-      </c>
-      <c r="J72" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K72" s="6">
-        <v>24.5</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I72">
+        <v>2</v>
+      </c>
+      <c r="J72">
+        <v>24.5</v>
+      </c>
+      <c r="K72">
+        <v>19.5</v>
+      </c>
+      <c r="L72">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>3</v>
       </c>
@@ -3867,23 +3695,26 @@
       <c r="F73" s="2">
         <v>72</v>
       </c>
-      <c r="G73" s="5">
+      <c r="G73">
         <v>13</v>
       </c>
-      <c r="H73" s="7">
-        <v>24.5</v>
-      </c>
-      <c r="I73" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="J73" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K73" s="6">
-        <v>24.5</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H73">
+        <v>24.5</v>
+      </c>
+      <c r="I73">
+        <v>23.5</v>
+      </c>
+      <c r="J73">
+        <v>24.5</v>
+      </c>
+      <c r="K73">
+        <v>12</v>
+      </c>
+      <c r="L73">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>3</v>
       </c>
@@ -3902,23 +3733,26 @@
       <c r="F74" s="2">
         <v>73</v>
       </c>
-      <c r="G74" s="5">
+      <c r="G74">
         <v>17</v>
       </c>
-      <c r="H74" s="5">
+      <c r="H74">
         <v>17</v>
       </c>
-      <c r="I74" s="5">
+      <c r="I74">
         <v>16</v>
       </c>
-      <c r="J74" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K74" s="6">
+      <c r="J74">
+        <v>24.5</v>
+      </c>
+      <c r="K74">
+        <v>19.5</v>
+      </c>
+      <c r="L74">
         <v>14</v>
       </c>
     </row>
-    <row r="75" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>3</v>
       </c>
@@ -3937,23 +3771,26 @@
       <c r="F75" s="2">
         <v>74</v>
       </c>
-      <c r="G75" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H75" s="7">
-        <v>24.5</v>
-      </c>
-      <c r="I75" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="J75" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K75" s="6">
-        <v>24.5</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G75">
+        <v>24.5</v>
+      </c>
+      <c r="H75">
+        <v>24.5</v>
+      </c>
+      <c r="I75">
+        <v>23.5</v>
+      </c>
+      <c r="J75">
+        <v>24.5</v>
+      </c>
+      <c r="K75">
+        <v>19.5</v>
+      </c>
+      <c r="L75">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>3</v>
       </c>
@@ -3972,23 +3809,26 @@
       <c r="F76" s="2">
         <v>75</v>
       </c>
-      <c r="G76" s="5">
+      <c r="G76">
         <v>7</v>
       </c>
-      <c r="H76" s="7">
-        <v>24.5</v>
-      </c>
-      <c r="I76" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="J76" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K76" s="6">
-        <v>24.5</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H76">
+        <v>24.5</v>
+      </c>
+      <c r="I76">
+        <v>23.5</v>
+      </c>
+      <c r="J76">
+        <v>24.5</v>
+      </c>
+      <c r="K76">
+        <v>12</v>
+      </c>
+      <c r="L76">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>3</v>
       </c>
@@ -4007,23 +3847,26 @@
       <c r="F77" s="2">
         <v>76</v>
       </c>
-      <c r="G77" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H77" s="5">
+      <c r="G77">
+        <v>24.5</v>
+      </c>
+      <c r="H77">
         <v>13</v>
       </c>
-      <c r="I77" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="J77" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K77" s="6">
-        <v>24.5</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I77">
+        <v>23.5</v>
+      </c>
+      <c r="J77">
+        <v>24.5</v>
+      </c>
+      <c r="K77">
+        <v>19.5</v>
+      </c>
+      <c r="L77">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>3</v>
       </c>
@@ -4042,23 +3885,26 @@
       <c r="F78" s="2">
         <v>77</v>
       </c>
-      <c r="G78" s="5">
+      <c r="G78">
         <v>15</v>
       </c>
-      <c r="H78" s="7">
-        <v>24.5</v>
-      </c>
-      <c r="I78" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="J78" s="6">
+      <c r="H78">
+        <v>24.5</v>
+      </c>
+      <c r="I78">
+        <v>23.5</v>
+      </c>
+      <c r="J78">
         <v>13</v>
       </c>
-      <c r="K78" s="6">
+      <c r="K78">
+        <v>19.5</v>
+      </c>
+      <c r="L78">
         <v>16</v>
       </c>
     </row>
-    <row r="79" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>3</v>
       </c>
@@ -4077,23 +3923,26 @@
       <c r="F79" s="2">
         <v>78</v>
       </c>
-      <c r="G79" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H79" s="7">
-        <v>24.5</v>
-      </c>
-      <c r="I79" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="J79" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K79" s="6">
+      <c r="G79">
+        <v>24.5</v>
+      </c>
+      <c r="H79">
+        <v>24.5</v>
+      </c>
+      <c r="I79">
+        <v>23.5</v>
+      </c>
+      <c r="J79">
+        <v>24.5</v>
+      </c>
+      <c r="K79">
+        <v>19.5</v>
+      </c>
+      <c r="L79">
         <v>17</v>
       </c>
     </row>
-    <row r="80" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>3</v>
       </c>
@@ -4112,23 +3961,26 @@
       <c r="F80" s="2">
         <v>79</v>
       </c>
-      <c r="G80" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H80" s="7">
-        <v>24.5</v>
-      </c>
-      <c r="I80" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="J80" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K80" s="6">
-        <v>24.5</v>
-      </c>
-    </row>
-    <row r="81" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G80">
+        <v>24.5</v>
+      </c>
+      <c r="H80">
+        <v>24.5</v>
+      </c>
+      <c r="I80">
+        <v>23.5</v>
+      </c>
+      <c r="J80">
+        <v>24.5</v>
+      </c>
+      <c r="K80">
+        <v>19.5</v>
+      </c>
+      <c r="L80">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>3</v>
       </c>
@@ -4147,23 +3999,26 @@
       <c r="F81" s="2">
         <v>80</v>
       </c>
-      <c r="G81" s="5">
+      <c r="G81">
         <v>14</v>
       </c>
-      <c r="H81" s="5">
+      <c r="H81">
         <v>17</v>
       </c>
-      <c r="I81" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="J81" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K81" s="6">
+      <c r="I81">
+        <v>23.5</v>
+      </c>
+      <c r="J81">
+        <v>24.5</v>
+      </c>
+      <c r="K81">
+        <v>19.5</v>
+      </c>
+      <c r="L81">
         <v>13</v>
       </c>
     </row>
-    <row r="82" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>3</v>
       </c>
@@ -4182,19 +4037,22 @@
       <c r="F82" s="2">
         <v>81</v>
       </c>
-      <c r="G82" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H82" s="7">
-        <v>24.5</v>
-      </c>
-      <c r="I82" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="J82" s="6">
-        <v>24.5</v>
-      </c>
-      <c r="K82" s="6">
+      <c r="G82">
+        <v>24.5</v>
+      </c>
+      <c r="H82">
+        <v>24.5</v>
+      </c>
+      <c r="I82">
+        <v>23.5</v>
+      </c>
+      <c r="J82">
+        <v>24.5</v>
+      </c>
+      <c r="K82">
+        <v>19.5</v>
+      </c>
+      <c r="L82">
         <v>17</v>
       </c>
     </row>
@@ -9919,7 +9777,7 @@
   <dimension ref="A1:EB26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10200,7 +10058,7 @@
         <v>1</v>
       </c>
       <c r="F3">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:132" x14ac:dyDescent="0.3">
@@ -10246,7 +10104,7 @@
         <v>3</v>
       </c>
       <c r="F5">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G5">
         <v>23</v>
@@ -10318,7 +10176,7 @@
         <v>3</v>
       </c>
       <c r="F8">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G8">
         <v>16</v>
@@ -10344,7 +10202,7 @@
         <v>1</v>
       </c>
       <c r="F9">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:132" x14ac:dyDescent="0.3">
@@ -10364,7 +10222,7 @@
         <v>3</v>
       </c>
       <c r="F10">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="G10">
         <v>13</v>
@@ -10416,7 +10274,7 @@
         <v>3</v>
       </c>
       <c r="F12">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:132" x14ac:dyDescent="0.3">
@@ -10436,7 +10294,7 @@
         <v>1</v>
       </c>
       <c r="F13">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H13">
         <v>6</v>
@@ -10462,7 +10320,7 @@
         <v>3</v>
       </c>
       <c r="F14">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H14">
         <v>4</v>
@@ -10485,7 +10343,7 @@
         <v>3</v>
       </c>
       <c r="F15">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J15">
         <v>7</v>
@@ -10534,7 +10392,7 @@
         <v>2</v>
       </c>
       <c r="F17">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H17">
         <v>2</v>
@@ -10557,7 +10415,7 @@
         <v>3</v>
       </c>
       <c r="F18">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -10577,7 +10435,7 @@
         <v>3</v>
       </c>
       <c r="F19">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
@@ -10597,7 +10455,7 @@
         <v>1</v>
       </c>
       <c r="F20">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
@@ -10617,7 +10475,7 @@
         <v>2</v>
       </c>
       <c r="F21">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
@@ -10637,7 +10495,7 @@
         <v>3</v>
       </c>
       <c r="F22">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
@@ -10677,12 +10535,7 @@
         <v>1</v>
       </c>
       <c r="F24">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F25">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>